<commit_message>
Cell References and error values
- handle getting values by cell reference <sheet>!<col><row>
- handle getting values by named cell ranges
- changed Cell#error_value to give better error information
</commit_message>
<xml_diff>
--- a/specs/data/various_samples.xlsx
+++ b/specs/data/various_samples.xlsx
@@ -4,16 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="140" windowWidth="21080" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="140" windowWidth="21080" windowHeight="9780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="text &amp; pic" sheetId="1" r:id="rId1"/>
     <sheet name="numbers" sheetId="2" r:id="rId2"/>
     <sheet name="dates" sheetId="3" r:id="rId3"/>
     <sheet name="bools &amp; errors" sheetId="4" r:id="rId4"/>
+    <sheet name="high refs" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="four_times_six">'high refs'!$AO$624</definedName>
     <definedName name="NAMES">'bools &amp; errors'!$D$2:$D$11</definedName>
+    <definedName name="nums">'high refs'!$AP$619:$AP$631</definedName>
   </definedNames>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>This</t>
   </si>
@@ -78,6 +81,10 @@
   </si>
   <si>
     <t>Booleans from Constants</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>This is some text</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -826,7 +833,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1073,7 +1079,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1088,7 +1093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1180,7 +1185,148 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="AM619:AP631"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="AE612" workbookViewId="0">
+      <selection activeCell="AO624" sqref="AO624"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="619" spans="39:42">
+      <c r="AM619" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO619">
+        <f>VLOOKUP(AP619, nums, 1,)*4</f>
+        <v>4</v>
+      </c>
+      <c r="AP619">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="620" spans="39:42">
+      <c r="AO620">
+        <f t="shared" ref="AO620:AO631" si="0">VLOOKUP(AP620, nums, 1,)*4</f>
+        <v>8</v>
+      </c>
+      <c r="AP620">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="621" spans="39:42">
+      <c r="AO621">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AP621">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="622" spans="39:42">
+      <c r="AO622">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="AP622">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="623" spans="39:42">
+      <c r="AO623">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="AP623">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="624" spans="39:42">
+      <c r="AO624">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="AP624">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="625" spans="41:42">
+      <c r="AO625">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AP625">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="626" spans="41:42">
+      <c r="AO626">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AP626">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="627" spans="41:42">
+      <c r="AO627">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="AP627">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="628" spans="41:42">
+      <c r="AO628">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AP628">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="629" spans="41:42">
+      <c r="AO629">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="AP629">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="630" spans="41:42">
+      <c r="AO630">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="AP630">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="631" spans="41:42">
+      <c r="AO631">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="AP631">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
improve handling of cells by reference
POI::Workbook can now answer an array of cells when the reference is an area (eg. 'dates!A2:A16')
</commit_message>
<xml_diff>
--- a/specs/data/various_samples.xlsx
+++ b/specs/data/various_samples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="140" windowWidth="21080" windowHeight="9780" activeTab="4"/>
+    <workbookView xWindow="340" yWindow="720" windowWidth="21080" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="text &amp; pic" sheetId="1" r:id="rId1"/>
@@ -537,10 +537,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -847,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1079,6 +1077,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1185,6 +1184,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1200,7 +1200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="AM619:AP631"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="AE612" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="AE612" workbookViewId="0">
       <selection activeCell="AO624" sqref="AO624"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
working on cell updates
</commit_message>
<xml_diff>
--- a/specs/data/various_samples.xlsx
+++ b/specs/data/various_samples.xlsx
@@ -92,13 +92,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="mmmm\ d\,\ yyyy"/>
     <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="171" formatCode="m/d"/>
+    <numFmt numFmtId="172" formatCode="dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -117,7 +119,6 @@
     <font>
       <sz val="8"/>
       <name val="Monaco"/>
-      <family val="3"/>
     </font>
     <font>
       <b/>
@@ -146,13 +147,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,6 +834,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -843,10 +847,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -854,9 +858,10 @@
     <col min="1" max="1" width="9.83203125" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -867,7 +872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>40237</v>
       </c>
@@ -879,8 +884,9 @@
         <f>B16</f>
         <v>40265</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <f>A2+1</f>
         <v>40238</v>
@@ -893,8 +899,9 @@
         <f t="shared" ref="C3:C16" si="0">C2+1</f>
         <v>40266</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <f t="shared" ref="A4:A16" si="1">A3+1</f>
         <v>40239</v>
@@ -908,7 +915,7 @@
         <v>40267</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <f t="shared" si="1"/>
         <v>40240</v>
@@ -922,7 +929,7 @@
         <v>40268</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" s="3">
         <f t="shared" si="1"/>
         <v>40241</v>
@@ -936,7 +943,7 @@
         <v>40269</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <f t="shared" si="1"/>
         <v>40242</v>
@@ -950,7 +957,7 @@
         <v>40270</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <f t="shared" si="1"/>
         <v>40243</v>
@@ -964,7 +971,7 @@
         <v>40271</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <f t="shared" si="1"/>
         <v>40244</v>
@@ -978,7 +985,7 @@
         <v>40272</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <f t="shared" si="1"/>
         <v>40245</v>
@@ -992,7 +999,7 @@
         <v>40273</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <f t="shared" si="1"/>
         <v>40246</v>
@@ -1006,7 +1013,7 @@
         <v>40274</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:5">
       <c r="A12" s="3">
         <f t="shared" si="1"/>
         <v>40247</v>
@@ -1020,7 +1027,7 @@
         <v>40275</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <f t="shared" si="1"/>
         <v>40248</v>
@@ -1034,7 +1041,7 @@
         <v>40276</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <f t="shared" si="1"/>
         <v>40249</v>
@@ -1048,7 +1055,7 @@
         <v>40277</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <f t="shared" si="1"/>
         <v>40250</v>
@@ -1062,7 +1069,7 @@
         <v>40278</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:5">
       <c r="A16" s="3">
         <f t="shared" si="1"/>
         <v>40251</v>
@@ -1327,6 +1334,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>